<commit_message>
updated data sources fpr all files
</commit_message>
<xml_diff>
--- a/0_Resources/Problems/6_Advanced _Data_Analytics/1_Analysis_Add-ins_Problem.xlsx
+++ b/0_Resources/Problems/6_Advanced _Data_Analytics/1_Analysis_Add-ins_Problem.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\OneDrive\Desktop\Projects\Excel_For_Data_Analytics\0_Resources\Problems\6_Advanced _Data_Analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\OneDrive\Desktop\Projects\Excel_For_Data_Analytics_1\Excel_Project_Data_Analytics\0_Resources\Problems\6_Advanced _Data_Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B942C749-F48C-4C6C-9E1E-2A66F772D38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3560258B-171F-479E-B879-23F737D4FAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{7520FE27-1537-4B08-B66C-E274CF35CCEC}"/>
   </bookViews>
@@ -66,7 +66,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -717,7 +717,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -759,24 +759,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="6" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,26 +784,31 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -898,7 +896,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5615D1E4-298D-462B-A8FD-6FA11FD526C5}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Result Cells" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5615D1E4-298D-462B-A8FD-6FA11FD526C5}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Result Cells" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -1316,10 +1314,10 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="50"/>
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
@@ -1415,10 +1413,10 @@
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="50"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="17" t="s">
@@ -1528,152 +1526,151 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" ht="16" x14ac:dyDescent="0.4">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="2:7" ht="16" x14ac:dyDescent="0.4">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="38" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="42" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="42" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="E4" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="39" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="34"/>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="25">
         <v>25</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="36">
         <v>25</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="36">
         <v>35</v>
       </c>
-      <c r="G6" s="39">
+      <c r="G6" s="36">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="34"/>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="25">
         <v>40</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="36">
         <v>40</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="36">
         <v>50</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="36">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="34"/>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="26">
         <v>2500</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="37">
         <v>2500</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="37">
         <v>3000</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="37">
         <v>2000</v>
       </c>
     </row>
     <row r="9" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="34"/>
-      <c r="C9" s="34" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="38">
         <v>4</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="38">
         <v>5</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="38">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
     </row>
     <row r="11" spans="2:7" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="36"/>
-      <c r="C11" s="36" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="27">
         <v>37500</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="27">
         <v>37500</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="27">
         <v>45000</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="27">
         <v>30000</v>
       </c>
     </row>
@@ -1714,242 +1711,241 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" ht="16" x14ac:dyDescent="0.4">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="2:7" ht="16" collapsed="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="38" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="42" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="42" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="E4" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="39" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="34"/>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="25">
         <v>25</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="36">
         <v>25</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="36">
         <v>35</v>
       </c>
-      <c r="G6" s="39">
+      <c r="G6" s="36">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="34"/>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="25">
         <v>40</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="36">
         <v>40</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="36">
         <v>50</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="36">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="34"/>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="26">
         <v>2500</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="37">
         <v>2500</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="37">
         <v>3000</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="37">
         <v>2000</v>
       </c>
     </row>
     <row r="9" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="34"/>
-      <c r="C9" s="34" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="38">
         <v>4</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F9" s="38">
         <v>5</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G9" s="38">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
     </row>
     <row r="11" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="34"/>
-      <c r="C11" s="34" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="25">
         <v>9375</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="25">
         <v>9375</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="25">
         <v>9000</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="25">
         <v>10000</v>
       </c>
     </row>
     <row r="12" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="34"/>
-      <c r="C12" s="34" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="25">
         <v>9375</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="25">
         <v>9375</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="25">
         <v>9000</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="25">
         <v>10000</v>
       </c>
     </row>
     <row r="13" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="34"/>
-      <c r="C13" s="34" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="25">
         <v>9375</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="25">
         <v>9375</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="25">
         <v>9000</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="25">
         <v>10000</v>
       </c>
     </row>
     <row r="14" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="34"/>
-      <c r="C14" s="34" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="25">
         <v>9375</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="25">
         <v>9375</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="25">
         <v>9000</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="34"/>
-      <c r="C15" s="34" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="25">
         <v>0</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="25">
         <v>0</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="25">
         <v>9000</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36" t="s">
+      <c r="B16" s="33"/>
+      <c r="C16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="27">
         <v>37500</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="27">
         <v>37500</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="27">
         <v>45000</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="27">
         <v>30000</v>
       </c>
     </row>
@@ -1978,7 +1974,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -1993,50 +1989,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="42" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="42" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="42" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="42" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="46"/>
+      <c r="A6" s="42"/>
       <c r="B6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="46"/>
+      <c r="A7" s="42"/>
       <c r="B7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="46"/>
+      <c r="A8" s="42"/>
       <c r="B8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="42" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2062,30 +2058,30 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="44" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="50">
+      <c r="D16" s="46">
         <v>60000</v>
       </c>
-      <c r="E16" s="50">
+      <c r="E16" s="46">
         <v>60000</v>
       </c>
     </row>
@@ -2095,53 +2091,53 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="48" t="s">
+      <c r="F20" s="44" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="51">
+      <c r="D21" s="47">
         <v>16.000299999999999</v>
       </c>
-      <c r="E21" s="51">
+      <c r="E21" s="47">
         <v>16.000299999999999</v>
       </c>
-      <c r="F21" s="49" t="s">
+      <c r="F21" s="45" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="52">
+      <c r="D22" s="48">
         <v>2500.03199754262</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="48">
         <v>2500.03199754262</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="43" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2151,82 +2147,82 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="48" t="s">
+      <c r="D26" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="48" t="s">
+      <c r="F26" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="G26" s="48" t="s">
+      <c r="G26" s="44" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="51">
+      <c r="D27" s="47">
         <v>60000</v>
       </c>
-      <c r="E27" s="49" t="s">
+      <c r="E27" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="49" t="s">
+      <c r="F27" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="49">
+      <c r="G27" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="51">
+      <c r="D28" s="47">
         <v>16</v>
       </c>
-      <c r="E28" s="49" t="s">
+      <c r="E28" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="49" t="s">
+      <c r="F28" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="49">
+      <c r="G28" s="45">
         <v>3.9996928275223915</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="52">
+      <c r="D29" s="48">
         <v>2500.03199754262</v>
       </c>
-      <c r="E29" s="47" t="s">
+      <c r="E29" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="47" t="s">
+      <c r="F29" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="47">
+      <c r="G29" s="43">
         <v>299.96800245737995</v>
       </c>
     </row>
@@ -2253,7 +2249,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
@@ -2261,7 +2257,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="40" t="s">
         <v>32</v>
       </c>
       <c r="B3" t="s">
@@ -2284,71 +2280,71 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4">
         <v>9375</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4">
         <v>9375</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4">
         <v>9375</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4">
         <v>9375</v>
       </c>
-      <c r="F4" s="45">
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" s="45">
+      <c r="G4">
         <v>37500</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5">
         <v>9000</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5">
         <v>9000</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5">
         <v>9000</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5">
         <v>9000</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5">
         <v>9000</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5">
         <v>45000</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6">
         <v>10000</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6">
         <v>10000</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6">
         <v>10000</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6">
         <v>30000</v>
       </c>
     </row>

</xml_diff>